<commit_message>
Edited TestData.xlsx and .gitignore
</commit_message>
<xml_diff>
--- a/ZavrsniProjekat/Docs/TestData.xlsx
+++ b/ZavrsniProjekat/Docs/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="287">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -486,10 +486,10 @@
     <t xml:space="preserve">Verify that user can’t submit future date as birthday date</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that user can’t submit date with year other than listed in year list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify that user can’t submit date with month other than listed in month list</t>
+    <t xml:space="preserve">Verify that user can’t submit date with invalid month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user can’t submit date with invalid day</t>
   </si>
   <si>
     <t xml:space="preserve">Verify that user can’t submit date with day other than listed in day table</t>
@@ -897,6 +897,9 @@
     <t xml:space="preserve">User stays on the same page, no popups or dialogs apear. ‘Date of Birth’ field is circled in red.</t>
   </si>
   <si>
+    <t xml:space="preserve">Verify that user can’t submit date with year earlier than listed in year list</t>
+  </si>
+  <si>
     <t xml:space="preserve">year = 1899</t>
   </si>
   <si>
@@ -1207,6 +1210,18 @@
   </si>
   <si>
     <t xml:space="preserve">Oct 1995 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1995 03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1995 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03 Oct 95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03 Oct 2101</t>
   </si>
 </sst>
 </file>
@@ -1697,12 +1712,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+      <selection pane="bottomLeft" activeCell="C52" activeCellId="0" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2484,6 +2499,9 @@
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
+      <c r="F42" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="9"/>
@@ -2492,6 +2510,9 @@
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
+      <c r="F43" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="9"/>
@@ -2500,6 +2521,9 @@
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
+      <c r="F44" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="9"/>
@@ -2508,6 +2532,9 @@
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
+      <c r="F45" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
@@ -2517,6 +2544,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="F46" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
@@ -2536,10 +2566,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D65" s="0"/>
-      <c r="E65" s="0"/>
-      <c r="H65" s="0" t="s">
+    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D64" s="0"/>
+      <c r="E64" s="0"/>
+      <c r="H64" s="0" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2569,7 +2599,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 F1">
+  <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>NOT(ISERROR(SEARCH("",F1)))</formula>
     </cfRule>
@@ -2598,9 +2628,9 @@
   <dimension ref="A1:H407"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A350" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="C357" activeCellId="0" sqref="C357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7844,7 +7874,7 @@
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B357" s="18"/>
       <c r="C357" s="19" t="s">
-        <v>54</v>
+        <v>178</v>
       </c>
       <c r="D357" s="20"/>
       <c r="E357" s="19"/>
@@ -8000,7 +8030,7 @@
         <v>92</v>
       </c>
       <c r="F368" s="24" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G368" s="23" t="s">
         <v>94</v>
@@ -8079,7 +8109,7 @@
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B374" s="18"/>
       <c r="C374" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D374" s="20"/>
       <c r="E374" s="19"/>
@@ -8235,7 +8265,7 @@
         <v>92</v>
       </c>
       <c r="F385" s="24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G385" s="23" t="s">
         <v>94</v>
@@ -8263,7 +8293,7 @@
         <v>97</v>
       </c>
       <c r="F387" s="24" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G387" s="23" t="s">
         <v>99</v>
@@ -8314,7 +8344,7 @@
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B391" s="18"/>
       <c r="C391" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D391" s="20"/>
       <c r="E391" s="19"/>
@@ -8470,7 +8500,7 @@
         <v>92</v>
       </c>
       <c r="F402" s="24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G402" s="23" t="s">
         <v>94</v>
@@ -8513,7 +8543,7 @@
         <v>100</v>
       </c>
       <c r="F405" s="24" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G405" s="23" t="s">
         <v>102</v>
@@ -8611,12 +8641,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+      <selection pane="bottomLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8637,388 +8667,408 @@
   <sheetData>
     <row r="1" s="37" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="37" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H1" s="37" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I1" s="37" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="38" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F2" s="38" t="n">
         <v>1234567890</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H2" s="38" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I2" s="38" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J2" s="38" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="K2" s="38" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="L2" s="38" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M2" s="38" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="N2" s="38" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F3" s="12" t="n">
         <v>123456789</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I5" s="0"/>
       <c r="L5" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="N5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I6" s="0"/>
       <c r="L6" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="12" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I7" s="0"/>
       <c r="L7" s="12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="I8" s="0"/>
       <c r="L8" s="12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="12" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="I9" s="0"/>
       <c r="L9" s="12" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I10" s="0"/>
       <c r="L10" s="12" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="36" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="I11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E12" s="36" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E13" s="36" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F13" s="0"/>
       <c r="G13" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="I13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E14" s="36" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E15" s="36" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G16" s="12" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G17" s="12" t="s">
-        <v>281</v>
+        <v>282</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="12" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="12" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="12" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
practice form, TestZavrsni, TOTOs
</commit_message>
<xml_diff>
--- a/ZavrsniProjekat/Docs/TestData.xlsx
+++ b/ZavrsniProjekat/Docs/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="309">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -927,6 +927,9 @@
     <t xml:space="preserve">date = 32</t>
   </si>
   <si>
+    <t xml:space="preserve">Verify that user can change years using date picker arrows</t>
+  </si>
+  <si>
     <t xml:space="preserve">Click on the arrow pointing left in the date picker box and continue clicking until previous year is displayed</t>
   </si>
   <si>
@@ -934,6 +937,9 @@
   </si>
   <si>
     <t xml:space="preserve">Date = 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected date visible in date picker field </t>
   </si>
   <si>
     <t xml:space="preserve">Click on the arrow pointing right in the date picker box and continue clicking until the next year is displayed</t>
@@ -1507,12 +1513,12 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
+      <selection pane="bottomLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="84.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="11.52"/>
@@ -2297,7 +2303,8 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E38" s="5" t="b">
+      <c r="E38" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F38" s="5" t="n">
@@ -2337,7 +2344,8 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E40" s="5" t="b">
+      <c r="E40" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F40" s="5" t="n">
@@ -2357,7 +2365,8 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E41" s="5" t="b">
+      <c r="E41" s="5" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="F41" s="5" t="n">
@@ -2941,13 +2950,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H523"/>
+  <dimension ref="A1:H514"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A396" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A403" activeCellId="0" sqref="A403"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A348" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B419" activeCellId="0" sqref="B419"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="11.54"/>
@@ -8828,7 +8837,7 @@
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B403" s="21"/>
       <c r="C403" s="34" t="s">
-        <v>51</v>
+        <v>288</v>
       </c>
       <c r="D403" s="23"/>
       <c r="E403" s="22"/>
@@ -8968,11 +8977,11 @@
       <c r="C413" s="25"/>
       <c r="D413" s="25"/>
       <c r="E413" s="26" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="F413" s="27"/>
       <c r="G413" s="26" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="H413" s="27"/>
     </row>
@@ -8984,92 +8993,92 @@
         <v>202</v>
       </c>
       <c r="F414" s="27" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G414" s="26" t="s">
         <v>204</v>
       </c>
       <c r="H414" s="27"/>
     </row>
-    <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B415" s="21"/>
-      <c r="C415" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D415" s="23"/>
-      <c r="E415" s="22"/>
-      <c r="F415" s="23"/>
-      <c r="G415" s="24"/>
-      <c r="H415" s="23"/>
-    </row>
-    <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="415" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B415" s="25"/>
+      <c r="C415" s="25"/>
+      <c r="D415" s="25"/>
+      <c r="E415" s="26" t="s">
+        <v>281</v>
+      </c>
+      <c r="F415" s="27"/>
+      <c r="G415" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="H415" s="27"/>
+    </row>
+    <row r="416" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B416" s="25"/>
       <c r="C416" s="25"/>
       <c r="D416" s="25"/>
       <c r="E416" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="F416" s="27" t="s">
-        <v>165</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="F416" s="27"/>
       <c r="G416" s="26" t="s">
-        <v>166</v>
+        <v>294</v>
       </c>
       <c r="H416" s="27"/>
     </row>
-    <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="417" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B417" s="25"/>
       <c r="C417" s="25"/>
       <c r="D417" s="25"/>
       <c r="E417" s="26" t="s">
-        <v>167</v>
+        <v>202</v>
       </c>
       <c r="F417" s="27" t="s">
-        <v>168</v>
+        <v>291</v>
       </c>
       <c r="G417" s="26" t="s">
-        <v>169</v>
+        <v>204</v>
       </c>
       <c r="H417" s="27"/>
     </row>
-    <row r="418" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B418" s="25"/>
-      <c r="C418" s="25"/>
-      <c r="D418" s="25"/>
-      <c r="E418" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="F418" s="27"/>
-      <c r="G418" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="H418" s="27"/>
-    </row>
-    <row r="419" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B418" s="21"/>
+      <c r="C418" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D418" s="23"/>
+      <c r="E418" s="22"/>
+      <c r="F418" s="23"/>
+      <c r="G418" s="24"/>
+      <c r="H418" s="23"/>
+    </row>
+    <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B419" s="25"/>
       <c r="C419" s="25"/>
       <c r="D419" s="25"/>
       <c r="E419" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="F419" s="27"/>
+        <v>164</v>
+      </c>
+      <c r="F419" s="27" t="s">
+        <v>165</v>
+      </c>
       <c r="G419" s="26" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="H419" s="27"/>
     </row>
-    <row r="420" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B420" s="25"/>
       <c r="C420" s="25"/>
       <c r="D420" s="25"/>
       <c r="E420" s="26" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="F420" s="27" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G420" s="26" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="H420" s="27"/>
     </row>
@@ -9078,13 +9087,11 @@
       <c r="C421" s="25"/>
       <c r="D421" s="25"/>
       <c r="E421" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="F421" s="27" t="s">
-        <v>178</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="F421" s="27"/>
       <c r="G421" s="26" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="H421" s="27"/>
     </row>
@@ -9093,11 +9100,11 @@
       <c r="C422" s="25"/>
       <c r="D422" s="25"/>
       <c r="E422" s="26" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F422" s="27"/>
       <c r="G422" s="26" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="H422" s="27"/>
     </row>
@@ -9106,39 +9113,41 @@
       <c r="C423" s="25"/>
       <c r="D423" s="25"/>
       <c r="E423" s="26" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F423" s="27" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G423" s="26" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="H423" s="27"/>
     </row>
-    <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="424" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B424" s="25"/>
       <c r="C424" s="25"/>
       <c r="D424" s="25"/>
       <c r="E424" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="F424" s="27"/>
+        <v>177</v>
+      </c>
+      <c r="F424" s="27" t="s">
+        <v>178</v>
+      </c>
       <c r="G424" s="26" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="H424" s="27"/>
     </row>
-    <row r="425" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="425" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B425" s="25"/>
       <c r="C425" s="25"/>
       <c r="D425" s="25"/>
       <c r="E425" s="26" t="s">
-        <v>291</v>
+        <v>180</v>
       </c>
       <c r="F425" s="27"/>
       <c r="G425" s="26" t="s">
-        <v>292</v>
+        <v>181</v>
       </c>
       <c r="H425" s="27"/>
     </row>
@@ -9147,110 +9156,106 @@
       <c r="C426" s="25"/>
       <c r="D426" s="25"/>
       <c r="E426" s="26" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="F426" s="27" t="s">
-        <v>290</v>
+        <v>183</v>
       </c>
       <c r="G426" s="26" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="H426" s="27"/>
     </row>
-    <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B427" s="21"/>
-      <c r="C427" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D427" s="23"/>
-      <c r="E427" s="22"/>
-      <c r="F427" s="23"/>
-      <c r="G427" s="24"/>
-      <c r="H427" s="23"/>
-    </row>
-    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="427" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B427" s="25"/>
+      <c r="C427" s="25"/>
+      <c r="D427" s="25"/>
+      <c r="E427" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="F427" s="27"/>
+      <c r="G427" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="H427" s="27"/>
+    </row>
+    <row r="428" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B428" s="25"/>
       <c r="C428" s="25"/>
       <c r="D428" s="25"/>
       <c r="E428" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="F428" s="27" t="s">
-        <v>165</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="F428" s="27"/>
       <c r="G428" s="26" t="s">
-        <v>166</v>
+        <v>297</v>
       </c>
       <c r="H428" s="27"/>
     </row>
-    <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="429" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B429" s="25"/>
       <c r="C429" s="25"/>
       <c r="D429" s="25"/>
       <c r="E429" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="F429" s="27" t="s">
-        <v>168</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="F429" s="27"/>
       <c r="G429" s="26" t="s">
-        <v>169</v>
+        <v>206</v>
       </c>
       <c r="H429" s="27"/>
     </row>
-    <row r="430" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="430" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B430" s="25"/>
       <c r="C430" s="25"/>
       <c r="D430" s="25"/>
       <c r="E430" s="26" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="F430" s="27"/>
       <c r="G430" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="H430" s="27"/>
-    </row>
-    <row r="431" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B431" s="25"/>
-      <c r="C431" s="25"/>
-      <c r="D431" s="25"/>
-      <c r="E431" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="F431" s="27"/>
-      <c r="G431" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="H431" s="27"/>
-    </row>
-    <row r="432" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>298</v>
+      </c>
+      <c r="H430" s="1"/>
+    </row>
+    <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B431" s="21"/>
+      <c r="C431" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D431" s="23"/>
+      <c r="E431" s="22"/>
+      <c r="F431" s="23"/>
+      <c r="G431" s="24"/>
+      <c r="H431" s="23"/>
+    </row>
+    <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B432" s="25"/>
       <c r="C432" s="25"/>
       <c r="D432" s="25"/>
       <c r="E432" s="26" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="F432" s="27" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G432" s="26" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="H432" s="27"/>
     </row>
-    <row r="433" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B433" s="25"/>
       <c r="C433" s="25"/>
       <c r="D433" s="25"/>
       <c r="E433" s="26" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="F433" s="27" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="G433" s="26" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="H433" s="27"/>
     </row>
@@ -9259,11 +9264,11 @@
       <c r="C434" s="25"/>
       <c r="D434" s="25"/>
       <c r="E434" s="26" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="F434" s="27"/>
       <c r="G434" s="26" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="H434" s="27"/>
     </row>
@@ -9272,13 +9277,11 @@
       <c r="C435" s="25"/>
       <c r="D435" s="25"/>
       <c r="E435" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="F435" s="27" t="s">
-        <v>183</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="F435" s="27"/>
       <c r="G435" s="26" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="H435" s="27"/>
     </row>
@@ -9287,11 +9290,13 @@
       <c r="C436" s="25"/>
       <c r="D436" s="25"/>
       <c r="E436" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="F436" s="27"/>
+        <v>174</v>
+      </c>
+      <c r="F436" s="27" t="s">
+        <v>175</v>
+      </c>
       <c r="G436" s="26" t="s">
-        <v>293</v>
+        <v>176</v>
       </c>
       <c r="H436" s="27"/>
     </row>
@@ -9300,11 +9305,13 @@
       <c r="C437" s="25"/>
       <c r="D437" s="25"/>
       <c r="E437" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="F437" s="27"/>
+        <v>177</v>
+      </c>
+      <c r="F437" s="27" t="s">
+        <v>178</v>
+      </c>
       <c r="G437" s="26" t="s">
-        <v>295</v>
+        <v>179</v>
       </c>
       <c r="H437" s="27"/>
     </row>
@@ -9313,65 +9320,67 @@
       <c r="C438" s="25"/>
       <c r="D438" s="25"/>
       <c r="E438" s="26" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="F438" s="27"/>
       <c r="G438" s="26" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="H438" s="27"/>
     </row>
-    <row r="439" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="439" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B439" s="25"/>
       <c r="C439" s="25"/>
       <c r="D439" s="25"/>
       <c r="E439" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="F439" s="27"/>
+        <v>182</v>
+      </c>
+      <c r="F439" s="27" t="s">
+        <v>183</v>
+      </c>
       <c r="G439" s="26" t="s">
-        <v>296</v>
-      </c>
-      <c r="H439" s="1"/>
-    </row>
-    <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B440" s="21"/>
-      <c r="C440" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="D440" s="23"/>
-      <c r="E440" s="22"/>
-      <c r="F440" s="23"/>
-      <c r="G440" s="24"/>
-      <c r="H440" s="23"/>
-    </row>
-    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>184</v>
+      </c>
+      <c r="H439" s="27"/>
+    </row>
+    <row r="440" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B440" s="25"/>
+      <c r="C440" s="25"/>
+      <c r="D440" s="25"/>
+      <c r="E440" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="F440" s="27"/>
+      <c r="G440" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="H440" s="27"/>
+    </row>
+    <row r="441" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B441" s="25"/>
       <c r="C441" s="25"/>
       <c r="D441" s="25"/>
       <c r="E441" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="F441" s="27" t="s">
-        <v>165</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="F441" s="27"/>
       <c r="G441" s="26" t="s">
-        <v>166</v>
+        <v>299</v>
       </c>
       <c r="H441" s="27"/>
     </row>
-    <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="442" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B442" s="25"/>
       <c r="C442" s="25"/>
       <c r="D442" s="25"/>
       <c r="E442" s="26" t="s">
-        <v>167</v>
+        <v>300</v>
       </c>
       <c r="F442" s="27" t="s">
-        <v>168</v>
+        <v>301</v>
       </c>
       <c r="G442" s="26" t="s">
-        <v>169</v>
+        <v>302</v>
       </c>
       <c r="H442" s="27"/>
     </row>
@@ -9380,67 +9389,65 @@
       <c r="C443" s="25"/>
       <c r="D443" s="25"/>
       <c r="E443" s="26" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="F443" s="27"/>
       <c r="G443" s="26" t="s">
-        <v>171</v>
+        <v>206</v>
       </c>
       <c r="H443" s="27"/>
     </row>
-    <row r="444" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="444" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B444" s="25"/>
       <c r="C444" s="25"/>
       <c r="D444" s="25"/>
       <c r="E444" s="26" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="F444" s="27"/>
       <c r="G444" s="26" t="s">
-        <v>173</v>
+        <v>303</v>
       </c>
       <c r="H444" s="27"/>
     </row>
-    <row r="445" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B445" s="25"/>
-      <c r="C445" s="25"/>
-      <c r="D445" s="25"/>
-      <c r="E445" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="F445" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="G445" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="H445" s="27"/>
-    </row>
-    <row r="446" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B445" s="21"/>
+      <c r="C445" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D445" s="23"/>
+      <c r="E445" s="22"/>
+      <c r="F445" s="23"/>
+      <c r="G445" s="24"/>
+      <c r="H445" s="23"/>
+    </row>
+    <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B446" s="25"/>
       <c r="C446" s="25"/>
       <c r="D446" s="25"/>
       <c r="E446" s="26" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="F446" s="27" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="G446" s="26" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="H446" s="27"/>
     </row>
-    <row r="447" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B447" s="25"/>
       <c r="C447" s="25"/>
       <c r="D447" s="25"/>
       <c r="E447" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="F447" s="27"/>
+        <v>167</v>
+      </c>
+      <c r="F447" s="27" t="s">
+        <v>168</v>
+      </c>
       <c r="G447" s="26" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="H447" s="27"/>
     </row>
@@ -9449,13 +9456,11 @@
       <c r="C448" s="25"/>
       <c r="D448" s="25"/>
       <c r="E448" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="F448" s="27" t="s">
-        <v>183</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="F448" s="27"/>
       <c r="G448" s="26" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H448" s="27"/>
     </row>
@@ -9464,11 +9469,11 @@
       <c r="C449" s="25"/>
       <c r="D449" s="25"/>
       <c r="E449" s="26" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="F449" s="27"/>
       <c r="G449" s="26" t="s">
-        <v>293</v>
+        <v>173</v>
       </c>
       <c r="H449" s="27"/>
     </row>
@@ -9477,11 +9482,13 @@
       <c r="C450" s="25"/>
       <c r="D450" s="25"/>
       <c r="E450" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="F450" s="27"/>
+        <v>174</v>
+      </c>
+      <c r="F450" s="27" t="s">
+        <v>175</v>
+      </c>
       <c r="G450" s="26" t="s">
-        <v>297</v>
+        <v>176</v>
       </c>
       <c r="H450" s="27"/>
     </row>
@@ -9490,13 +9497,13 @@
       <c r="C451" s="25"/>
       <c r="D451" s="25"/>
       <c r="E451" s="26" t="s">
-        <v>298</v>
+        <v>177</v>
       </c>
       <c r="F451" s="27" t="s">
-        <v>299</v>
+        <v>178</v>
       </c>
       <c r="G451" s="26" t="s">
-        <v>300</v>
+        <v>179</v>
       </c>
       <c r="H451" s="27"/>
     </row>
@@ -9505,65 +9512,67 @@
       <c r="C452" s="25"/>
       <c r="D452" s="25"/>
       <c r="E452" s="26" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="F452" s="27"/>
       <c r="G452" s="26" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="H452" s="27"/>
     </row>
-    <row r="453" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="453" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B453" s="25"/>
       <c r="C453" s="25"/>
       <c r="D453" s="25"/>
       <c r="E453" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="F453" s="27"/>
+        <v>182</v>
+      </c>
+      <c r="F453" s="27" t="s">
+        <v>183</v>
+      </c>
       <c r="G453" s="26" t="s">
-        <v>301</v>
+        <v>184</v>
       </c>
       <c r="H453" s="27"/>
     </row>
-    <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B454" s="21"/>
-      <c r="C454" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="D454" s="23"/>
-      <c r="E454" s="22"/>
-      <c r="F454" s="23"/>
-      <c r="G454" s="24"/>
-      <c r="H454" s="23"/>
-    </row>
-    <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="454" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B454" s="25"/>
+      <c r="C454" s="25"/>
+      <c r="D454" s="25"/>
+      <c r="E454" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="F454" s="27"/>
+      <c r="G454" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="H454" s="27"/>
+    </row>
+    <row r="455" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B455" s="25"/>
       <c r="C455" s="25"/>
       <c r="D455" s="25"/>
       <c r="E455" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="F455" s="27" t="s">
-        <v>165</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="F455" s="27"/>
       <c r="G455" s="26" t="s">
-        <v>166</v>
+        <v>299</v>
       </c>
       <c r="H455" s="27"/>
     </row>
-    <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="456" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B456" s="25"/>
       <c r="C456" s="25"/>
       <c r="D456" s="25"/>
       <c r="E456" s="26" t="s">
-        <v>167</v>
+        <v>300</v>
       </c>
       <c r="F456" s="27" t="s">
-        <v>168</v>
+        <v>304</v>
       </c>
       <c r="G456" s="26" t="s">
-        <v>169</v>
+        <v>302</v>
       </c>
       <c r="H456" s="27"/>
     </row>
@@ -9572,67 +9581,65 @@
       <c r="C457" s="25"/>
       <c r="D457" s="25"/>
       <c r="E457" s="26" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="F457" s="27"/>
       <c r="G457" s="26" t="s">
-        <v>171</v>
+        <v>206</v>
       </c>
       <c r="H457" s="27"/>
     </row>
-    <row r="458" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="458" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B458" s="25"/>
       <c r="C458" s="25"/>
       <c r="D458" s="25"/>
       <c r="E458" s="26" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="F458" s="27"/>
       <c r="G458" s="26" t="s">
-        <v>173</v>
+        <v>303</v>
       </c>
       <c r="H458" s="27"/>
     </row>
-    <row r="459" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B459" s="25"/>
-      <c r="C459" s="25"/>
-      <c r="D459" s="25"/>
-      <c r="E459" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="F459" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="G459" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="H459" s="27"/>
-    </row>
-    <row r="460" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B459" s="21"/>
+      <c r="C459" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D459" s="23"/>
+      <c r="E459" s="22"/>
+      <c r="F459" s="23"/>
+      <c r="G459" s="24"/>
+      <c r="H459" s="23"/>
+    </row>
+    <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B460" s="25"/>
       <c r="C460" s="25"/>
       <c r="D460" s="25"/>
       <c r="E460" s="26" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="F460" s="27" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="G460" s="26" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="H460" s="27"/>
     </row>
-    <row r="461" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B461" s="25"/>
       <c r="C461" s="25"/>
       <c r="D461" s="25"/>
       <c r="E461" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="F461" s="27"/>
+        <v>167</v>
+      </c>
+      <c r="F461" s="27" t="s">
+        <v>168</v>
+      </c>
       <c r="G461" s="26" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="H461" s="27"/>
     </row>
@@ -9641,13 +9648,11 @@
       <c r="C462" s="25"/>
       <c r="D462" s="25"/>
       <c r="E462" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="F462" s="27" t="s">
-        <v>183</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="F462" s="27"/>
       <c r="G462" s="26" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H462" s="27"/>
     </row>
@@ -9656,11 +9661,11 @@
       <c r="C463" s="25"/>
       <c r="D463" s="25"/>
       <c r="E463" s="26" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="F463" s="27"/>
       <c r="G463" s="26" t="s">
-        <v>293</v>
+        <v>173</v>
       </c>
       <c r="H463" s="27"/>
     </row>
@@ -9669,11 +9674,13 @@
       <c r="C464" s="25"/>
       <c r="D464" s="25"/>
       <c r="E464" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="F464" s="27"/>
+        <v>174</v>
+      </c>
+      <c r="F464" s="27" t="s">
+        <v>175</v>
+      </c>
       <c r="G464" s="26" t="s">
-        <v>297</v>
+        <v>176</v>
       </c>
       <c r="H464" s="27"/>
     </row>
@@ -9682,13 +9689,13 @@
       <c r="C465" s="25"/>
       <c r="D465" s="25"/>
       <c r="E465" s="26" t="s">
-        <v>298</v>
+        <v>177</v>
       </c>
       <c r="F465" s="27" t="s">
-        <v>302</v>
+        <v>178</v>
       </c>
       <c r="G465" s="26" t="s">
-        <v>300</v>
+        <v>179</v>
       </c>
       <c r="H465" s="27"/>
     </row>
@@ -9697,65 +9704,67 @@
       <c r="C466" s="25"/>
       <c r="D466" s="25"/>
       <c r="E466" s="26" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="F466" s="27"/>
       <c r="G466" s="26" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="H466" s="27"/>
     </row>
-    <row r="467" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="467" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B467" s="25"/>
       <c r="C467" s="25"/>
       <c r="D467" s="25"/>
       <c r="E467" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="F467" s="27"/>
+        <v>182</v>
+      </c>
+      <c r="F467" s="27" t="s">
+        <v>183</v>
+      </c>
       <c r="G467" s="26" t="s">
-        <v>301</v>
+        <v>184</v>
       </c>
       <c r="H467" s="27"/>
     </row>
-    <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B468" s="21"/>
-      <c r="C468" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="D468" s="23"/>
-      <c r="E468" s="22"/>
-      <c r="F468" s="23"/>
-      <c r="G468" s="24"/>
-      <c r="H468" s="23"/>
-    </row>
-    <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="468" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B468" s="25"/>
+      <c r="C468" s="25"/>
+      <c r="D468" s="25"/>
+      <c r="E468" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="F468" s="27"/>
+      <c r="G468" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="H468" s="27"/>
+    </row>
+    <row r="469" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B469" s="25"/>
       <c r="C469" s="25"/>
       <c r="D469" s="25"/>
       <c r="E469" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="F469" s="27" t="s">
-        <v>165</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="F469" s="27"/>
       <c r="G469" s="26" t="s">
-        <v>166</v>
+        <v>299</v>
       </c>
       <c r="H469" s="27"/>
     </row>
-    <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="470" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B470" s="25"/>
       <c r="C470" s="25"/>
       <c r="D470" s="25"/>
       <c r="E470" s="26" t="s">
-        <v>167</v>
+        <v>300</v>
       </c>
       <c r="F470" s="27" t="s">
-        <v>168</v>
+        <v>305</v>
       </c>
       <c r="G470" s="26" t="s">
-        <v>169</v>
+        <v>302</v>
       </c>
       <c r="H470" s="27"/>
     </row>
@@ -9764,67 +9773,65 @@
       <c r="C471" s="25"/>
       <c r="D471" s="25"/>
       <c r="E471" s="26" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="F471" s="27"/>
       <c r="G471" s="26" t="s">
-        <v>171</v>
+        <v>206</v>
       </c>
       <c r="H471" s="27"/>
     </row>
-    <row r="472" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="472" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B472" s="25"/>
       <c r="C472" s="25"/>
       <c r="D472" s="25"/>
       <c r="E472" s="26" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="F472" s="27"/>
       <c r="G472" s="26" t="s">
-        <v>173</v>
+        <v>303</v>
       </c>
       <c r="H472" s="27"/>
     </row>
-    <row r="473" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B473" s="25"/>
-      <c r="C473" s="25"/>
-      <c r="D473" s="25"/>
-      <c r="E473" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="F473" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="G473" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="H473" s="27"/>
-    </row>
-    <row r="474" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B473" s="21"/>
+      <c r="C473" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D473" s="23"/>
+      <c r="E473" s="22"/>
+      <c r="F473" s="23"/>
+      <c r="G473" s="24"/>
+      <c r="H473" s="23"/>
+    </row>
+    <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B474" s="25"/>
       <c r="C474" s="25"/>
       <c r="D474" s="25"/>
       <c r="E474" s="26" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="F474" s="27" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="G474" s="26" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="H474" s="27"/>
     </row>
-    <row r="475" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B475" s="25"/>
       <c r="C475" s="25"/>
       <c r="D475" s="25"/>
       <c r="E475" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="F475" s="27"/>
+        <v>167</v>
+      </c>
+      <c r="F475" s="27" t="s">
+        <v>168</v>
+      </c>
       <c r="G475" s="26" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="H475" s="27"/>
     </row>
@@ -9833,13 +9840,11 @@
       <c r="C476" s="25"/>
       <c r="D476" s="25"/>
       <c r="E476" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="F476" s="27" t="s">
-        <v>183</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="F476" s="27"/>
       <c r="G476" s="26" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H476" s="27"/>
     </row>
@@ -9848,11 +9853,11 @@
       <c r="C477" s="25"/>
       <c r="D477" s="25"/>
       <c r="E477" s="26" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="F477" s="27"/>
       <c r="G477" s="26" t="s">
-        <v>293</v>
+        <v>173</v>
       </c>
       <c r="H477" s="27"/>
     </row>
@@ -9861,11 +9866,13 @@
       <c r="C478" s="25"/>
       <c r="D478" s="25"/>
       <c r="E478" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="F478" s="27"/>
+        <v>174</v>
+      </c>
+      <c r="F478" s="27" t="s">
+        <v>175</v>
+      </c>
       <c r="G478" s="26" t="s">
-        <v>297</v>
+        <v>176</v>
       </c>
       <c r="H478" s="27"/>
     </row>
@@ -9874,13 +9881,13 @@
       <c r="C479" s="25"/>
       <c r="D479" s="25"/>
       <c r="E479" s="26" t="s">
-        <v>298</v>
+        <v>177</v>
       </c>
       <c r="F479" s="27" t="s">
-        <v>303</v>
+        <v>178</v>
       </c>
       <c r="G479" s="26" t="s">
-        <v>300</v>
+        <v>179</v>
       </c>
       <c r="H479" s="27"/>
     </row>
@@ -9889,65 +9896,67 @@
       <c r="C480" s="25"/>
       <c r="D480" s="25"/>
       <c r="E480" s="26" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="F480" s="27"/>
       <c r="G480" s="26" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="H480" s="27"/>
     </row>
-    <row r="481" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="481" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B481" s="25"/>
       <c r="C481" s="25"/>
       <c r="D481" s="25"/>
       <c r="E481" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="F481" s="27"/>
+        <v>182</v>
+      </c>
+      <c r="F481" s="27" t="s">
+        <v>183</v>
+      </c>
       <c r="G481" s="26" t="s">
-        <v>301</v>
+        <v>184</v>
       </c>
       <c r="H481" s="27"/>
     </row>
-    <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B482" s="21"/>
-      <c r="C482" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="D482" s="23"/>
-      <c r="E482" s="22"/>
-      <c r="F482" s="23"/>
-      <c r="G482" s="24"/>
-      <c r="H482" s="23"/>
-    </row>
-    <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="482" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B482" s="25"/>
+      <c r="C482" s="25"/>
+      <c r="D482" s="25"/>
+      <c r="E482" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="F482" s="27"/>
+      <c r="G482" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="H482" s="27"/>
+    </row>
+    <row r="483" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B483" s="25"/>
       <c r="C483" s="25"/>
       <c r="D483" s="25"/>
       <c r="E483" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="F483" s="27" t="s">
-        <v>165</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="F483" s="27"/>
       <c r="G483" s="26" t="s">
-        <v>166</v>
+        <v>299</v>
       </c>
       <c r="H483" s="27"/>
     </row>
-    <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="484" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B484" s="25"/>
       <c r="C484" s="25"/>
       <c r="D484" s="25"/>
       <c r="E484" s="26" t="s">
-        <v>167</v>
+        <v>300</v>
       </c>
       <c r="F484" s="27" t="s">
-        <v>168</v>
+        <v>306</v>
       </c>
       <c r="G484" s="26" t="s">
-        <v>169</v>
+        <v>302</v>
       </c>
       <c r="H484" s="27"/>
     </row>
@@ -9956,67 +9965,65 @@
       <c r="C485" s="25"/>
       <c r="D485" s="25"/>
       <c r="E485" s="26" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="F485" s="27"/>
       <c r="G485" s="26" t="s">
-        <v>171</v>
+        <v>206</v>
       </c>
       <c r="H485" s="27"/>
     </row>
-    <row r="486" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="486" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B486" s="25"/>
       <c r="C486" s="25"/>
       <c r="D486" s="25"/>
       <c r="E486" s="26" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="F486" s="27"/>
       <c r="G486" s="26" t="s">
-        <v>173</v>
+        <v>303</v>
       </c>
       <c r="H486" s="27"/>
     </row>
-    <row r="487" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B487" s="25"/>
-      <c r="C487" s="25"/>
-      <c r="D487" s="25"/>
-      <c r="E487" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="F487" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="G487" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="H487" s="27"/>
-    </row>
-    <row r="488" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B487" s="21"/>
+      <c r="C487" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D487" s="23"/>
+      <c r="E487" s="22"/>
+      <c r="F487" s="23"/>
+      <c r="G487" s="24"/>
+      <c r="H487" s="23"/>
+    </row>
+    <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B488" s="25"/>
       <c r="C488" s="25"/>
       <c r="D488" s="25"/>
       <c r="E488" s="26" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="F488" s="27" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="G488" s="26" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="H488" s="27"/>
     </row>
-    <row r="489" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B489" s="25"/>
       <c r="C489" s="25"/>
       <c r="D489" s="25"/>
       <c r="E489" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="F489" s="27"/>
+        <v>167</v>
+      </c>
+      <c r="F489" s="27" t="s">
+        <v>168</v>
+      </c>
       <c r="G489" s="26" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="H489" s="27"/>
     </row>
@@ -10025,13 +10032,11 @@
       <c r="C490" s="25"/>
       <c r="D490" s="25"/>
       <c r="E490" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="F490" s="27" t="s">
-        <v>183</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="F490" s="27"/>
       <c r="G490" s="26" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H490" s="27"/>
     </row>
@@ -10040,11 +10045,11 @@
       <c r="C491" s="25"/>
       <c r="D491" s="25"/>
       <c r="E491" s="26" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="F491" s="27"/>
       <c r="G491" s="26" t="s">
-        <v>293</v>
+        <v>173</v>
       </c>
       <c r="H491" s="27"/>
     </row>
@@ -10053,11 +10058,13 @@
       <c r="C492" s="25"/>
       <c r="D492" s="25"/>
       <c r="E492" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="F492" s="27"/>
+        <v>174</v>
+      </c>
+      <c r="F492" s="27" t="s">
+        <v>175</v>
+      </c>
       <c r="G492" s="26" t="s">
-        <v>297</v>
+        <v>176</v>
       </c>
       <c r="H492" s="27"/>
     </row>
@@ -10066,13 +10073,13 @@
       <c r="C493" s="25"/>
       <c r="D493" s="25"/>
       <c r="E493" s="26" t="s">
-        <v>298</v>
+        <v>177</v>
       </c>
       <c r="F493" s="27" t="s">
-        <v>304</v>
+        <v>178</v>
       </c>
       <c r="G493" s="26" t="s">
-        <v>300</v>
+        <v>179</v>
       </c>
       <c r="H493" s="27"/>
     </row>
@@ -10081,65 +10088,67 @@
       <c r="C494" s="25"/>
       <c r="D494" s="25"/>
       <c r="E494" s="26" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="F494" s="27"/>
       <c r="G494" s="26" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="H494" s="27"/>
     </row>
-    <row r="495" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="495" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B495" s="25"/>
       <c r="C495" s="25"/>
       <c r="D495" s="25"/>
       <c r="E495" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="F495" s="27"/>
+        <v>182</v>
+      </c>
+      <c r="F495" s="27" t="s">
+        <v>183</v>
+      </c>
       <c r="G495" s="26" t="s">
-        <v>301</v>
+        <v>184</v>
       </c>
       <c r="H495" s="27"/>
     </row>
-    <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B496" s="21"/>
-      <c r="C496" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="D496" s="23"/>
-      <c r="E496" s="22"/>
-      <c r="F496" s="23"/>
-      <c r="G496" s="24"/>
-      <c r="H496" s="23"/>
-    </row>
-    <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="496" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B496" s="25"/>
+      <c r="C496" s="25"/>
+      <c r="D496" s="25"/>
+      <c r="E496" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="F496" s="27"/>
+      <c r="G496" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="H496" s="27"/>
+    </row>
+    <row r="497" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B497" s="25"/>
       <c r="C497" s="25"/>
       <c r="D497" s="25"/>
       <c r="E497" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="F497" s="27" t="s">
-        <v>165</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="F497" s="27"/>
       <c r="G497" s="26" t="s">
-        <v>166</v>
+        <v>299</v>
       </c>
       <c r="H497" s="27"/>
     </row>
-    <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="498" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B498" s="25"/>
       <c r="C498" s="25"/>
       <c r="D498" s="25"/>
       <c r="E498" s="26" t="s">
-        <v>167</v>
+        <v>300</v>
       </c>
       <c r="F498" s="27" t="s">
-        <v>168</v>
+        <v>307</v>
       </c>
       <c r="G498" s="26" t="s">
-        <v>169</v>
+        <v>302</v>
       </c>
       <c r="H498" s="27"/>
     </row>
@@ -10148,67 +10157,65 @@
       <c r="C499" s="25"/>
       <c r="D499" s="25"/>
       <c r="E499" s="26" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="F499" s="27"/>
       <c r="G499" s="26" t="s">
-        <v>171</v>
+        <v>206</v>
       </c>
       <c r="H499" s="27"/>
     </row>
-    <row r="500" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="500" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B500" s="25"/>
       <c r="C500" s="25"/>
       <c r="D500" s="25"/>
       <c r="E500" s="26" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="F500" s="27"/>
       <c r="G500" s="26" t="s">
-        <v>173</v>
+        <v>303</v>
       </c>
       <c r="H500" s="27"/>
     </row>
-    <row r="501" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B501" s="25"/>
-      <c r="C501" s="25"/>
-      <c r="D501" s="25"/>
-      <c r="E501" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="F501" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="G501" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="H501" s="27"/>
-    </row>
-    <row r="502" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B501" s="21"/>
+      <c r="C501" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="D501" s="23"/>
+      <c r="E501" s="22"/>
+      <c r="F501" s="23"/>
+      <c r="G501" s="24"/>
+      <c r="H501" s="23"/>
+    </row>
+    <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B502" s="25"/>
       <c r="C502" s="25"/>
       <c r="D502" s="25"/>
       <c r="E502" s="26" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="F502" s="27" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="G502" s="26" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="H502" s="27"/>
     </row>
-    <row r="503" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B503" s="25"/>
       <c r="C503" s="25"/>
       <c r="D503" s="25"/>
       <c r="E503" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="F503" s="27"/>
+        <v>167</v>
+      </c>
+      <c r="F503" s="27" t="s">
+        <v>168</v>
+      </c>
       <c r="G503" s="26" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="H503" s="27"/>
     </row>
@@ -10217,13 +10224,11 @@
       <c r="C504" s="25"/>
       <c r="D504" s="25"/>
       <c r="E504" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="F504" s="27" t="s">
-        <v>183</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="F504" s="27"/>
       <c r="G504" s="26" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H504" s="27"/>
     </row>
@@ -10232,11 +10237,11 @@
       <c r="C505" s="25"/>
       <c r="D505" s="25"/>
       <c r="E505" s="26" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="F505" s="27"/>
       <c r="G505" s="26" t="s">
-        <v>293</v>
+        <v>173</v>
       </c>
       <c r="H505" s="27"/>
     </row>
@@ -10245,11 +10250,13 @@
       <c r="C506" s="25"/>
       <c r="D506" s="25"/>
       <c r="E506" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="F506" s="27"/>
+        <v>174</v>
+      </c>
+      <c r="F506" s="27" t="s">
+        <v>175</v>
+      </c>
       <c r="G506" s="26" t="s">
-        <v>297</v>
+        <v>176</v>
       </c>
       <c r="H506" s="27"/>
     </row>
@@ -10258,13 +10265,13 @@
       <c r="C507" s="25"/>
       <c r="D507" s="25"/>
       <c r="E507" s="26" t="s">
-        <v>298</v>
+        <v>177</v>
       </c>
       <c r="F507" s="27" t="s">
-        <v>305</v>
+        <v>178</v>
       </c>
       <c r="G507" s="26" t="s">
-        <v>300</v>
+        <v>179</v>
       </c>
       <c r="H507" s="27"/>
     </row>
@@ -10273,65 +10280,67 @@
       <c r="C508" s="25"/>
       <c r="D508" s="25"/>
       <c r="E508" s="26" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
       <c r="F508" s="27"/>
       <c r="G508" s="26" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="H508" s="27"/>
     </row>
-    <row r="509" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="509" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B509" s="25"/>
       <c r="C509" s="25"/>
       <c r="D509" s="25"/>
       <c r="E509" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="F509" s="27"/>
+        <v>182</v>
+      </c>
+      <c r="F509" s="27" t="s">
+        <v>183</v>
+      </c>
       <c r="G509" s="26" t="s">
-        <v>301</v>
+        <v>184</v>
       </c>
       <c r="H509" s="27"/>
     </row>
-    <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B510" s="21"/>
-      <c r="C510" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="D510" s="23"/>
-      <c r="E510" s="22"/>
-      <c r="F510" s="23"/>
-      <c r="G510" s="24"/>
-      <c r="H510" s="23"/>
-    </row>
-    <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="510" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B510" s="25"/>
+      <c r="C510" s="25"/>
+      <c r="D510" s="25"/>
+      <c r="E510" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="F510" s="27"/>
+      <c r="G510" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="H510" s="27"/>
+    </row>
+    <row r="511" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B511" s="25"/>
       <c r="C511" s="25"/>
       <c r="D511" s="25"/>
       <c r="E511" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="F511" s="27" t="s">
-        <v>165</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="F511" s="27"/>
       <c r="G511" s="26" t="s">
-        <v>166</v>
+        <v>299</v>
       </c>
       <c r="H511" s="27"/>
     </row>
-    <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="512" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B512" s="25"/>
       <c r="C512" s="25"/>
       <c r="D512" s="25"/>
       <c r="E512" s="26" t="s">
-        <v>167</v>
+        <v>300</v>
       </c>
       <c r="F512" s="27" t="s">
-        <v>168</v>
+        <v>308</v>
       </c>
       <c r="G512" s="26" t="s">
-        <v>169</v>
+        <v>302</v>
       </c>
       <c r="H512" s="27"/>
     </row>
@@ -10340,154 +10349,29 @@
       <c r="C513" s="25"/>
       <c r="D513" s="25"/>
       <c r="E513" s="26" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="F513" s="27"/>
       <c r="G513" s="26" t="s">
-        <v>171</v>
+        <v>206</v>
       </c>
       <c r="H513" s="27"/>
     </row>
-    <row r="514" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="514" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B514" s="25"/>
       <c r="C514" s="25"/>
       <c r="D514" s="25"/>
       <c r="E514" s="26" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="F514" s="27"/>
       <c r="G514" s="26" t="s">
-        <v>173</v>
+        <v>298</v>
       </c>
       <c r="H514" s="27"/>
     </row>
-    <row r="515" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B515" s="25"/>
-      <c r="C515" s="25"/>
-      <c r="D515" s="25"/>
-      <c r="E515" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="F515" s="27" t="s">
-        <v>175</v>
-      </c>
-      <c r="G515" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="H515" s="27"/>
-    </row>
-    <row r="516" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B516" s="25"/>
-      <c r="C516" s="25"/>
-      <c r="D516" s="25"/>
-      <c r="E516" s="26" t="s">
-        <v>177</v>
-      </c>
-      <c r="F516" s="27" t="s">
-        <v>178</v>
-      </c>
-      <c r="G516" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="H516" s="27"/>
-    </row>
-    <row r="517" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B517" s="25"/>
-      <c r="C517" s="25"/>
-      <c r="D517" s="25"/>
-      <c r="E517" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="F517" s="27"/>
-      <c r="G517" s="26" t="s">
-        <v>181</v>
-      </c>
-      <c r="H517" s="27"/>
-    </row>
-    <row r="518" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B518" s="25"/>
-      <c r="C518" s="25"/>
-      <c r="D518" s="25"/>
-      <c r="E518" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="F518" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="G518" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="H518" s="27"/>
-    </row>
-    <row r="519" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B519" s="25"/>
-      <c r="C519" s="25"/>
-      <c r="D519" s="25"/>
-      <c r="E519" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="F519" s="27"/>
-      <c r="G519" s="26" t="s">
-        <v>293</v>
-      </c>
-      <c r="H519" s="27"/>
-    </row>
-    <row r="520" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B520" s="25"/>
-      <c r="C520" s="25"/>
-      <c r="D520" s="25"/>
-      <c r="E520" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="F520" s="27"/>
-      <c r="G520" s="26" t="s">
-        <v>297</v>
-      </c>
-      <c r="H520" s="27"/>
-    </row>
-    <row r="521" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B521" s="25"/>
-      <c r="C521" s="25"/>
-      <c r="D521" s="25"/>
-      <c r="E521" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="F521" s="27" t="s">
-        <v>306</v>
-      </c>
-      <c r="G521" s="26" t="s">
-        <v>300</v>
-      </c>
-      <c r="H521" s="27"/>
-    </row>
-    <row r="522" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B522" s="25"/>
-      <c r="C522" s="25"/>
-      <c r="D522" s="25"/>
-      <c r="E522" s="26" t="s">
-        <v>205</v>
-      </c>
-      <c r="F522" s="27"/>
-      <c r="G522" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="H522" s="27"/>
-    </row>
-    <row r="523" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B523" s="25"/>
-      <c r="C523" s="25"/>
-      <c r="D523" s="25"/>
-      <c r="E523" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="F523" s="27"/>
-      <c r="G523" s="26" t="s">
-        <v>296</v>
-      </c>
-      <c r="H523" s="27"/>
-    </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="45">
     <mergeCell ref="A2:A44"/>
     <mergeCell ref="B3:D11"/>
     <mergeCell ref="B13:D42"/>
@@ -10525,15 +10409,14 @@
     <mergeCell ref="B356:D370"/>
     <mergeCell ref="B372:D386"/>
     <mergeCell ref="B388:D402"/>
-    <mergeCell ref="B404:D414"/>
-    <mergeCell ref="B416:D426"/>
-    <mergeCell ref="B428:D439"/>
-    <mergeCell ref="B441:D453"/>
-    <mergeCell ref="B455:D467"/>
-    <mergeCell ref="B469:D481"/>
-    <mergeCell ref="B483:D495"/>
-    <mergeCell ref="B497:D509"/>
-    <mergeCell ref="B511:D523"/>
+    <mergeCell ref="B404:D417"/>
+    <mergeCell ref="B419:D430"/>
+    <mergeCell ref="B432:D444"/>
+    <mergeCell ref="B446:D458"/>
+    <mergeCell ref="B460:D472"/>
+    <mergeCell ref="B474:D486"/>
+    <mergeCell ref="B488:D500"/>
+    <mergeCell ref="B502:D514"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F19" r:id="rId1" display="email = imeprezime@domen.com"/>

</xml_diff>